<commit_message>
+4 +4 m4 stocks
</commit_message>
<xml_diff>
--- a/changes/m4-stocks.xlsx
+++ b/changes/m4-stocks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lingl\Documents\deadline-balancing\changes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39DA351B-F672-48DA-B167-0A4AECE4341B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B7B0B7AE-6C63-41AE-AA5A-5618BA0132ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1239,8 +1239,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F53" sqref="F53"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1325,17 +1325,17 @@
         <v>0.32</v>
       </c>
       <c r="E3" s="1">
-        <v>-9</v>
+        <v>-7</v>
       </c>
       <c r="F3" s="1">
-        <v>-13</v>
+        <v>-11</v>
       </c>
       <c r="M3" s="1">
         <v>1500</v>
       </c>
       <c r="N3" s="1">
         <f>C3-(D3*20)-(E3*0.8)-(F3*0.6)-(H3*5)</f>
-        <v>18.600000000000001</v>
+        <v>15.799999999999999</v>
       </c>
       <c r="P3" s="1">
         <v>19</v>
@@ -1445,17 +1445,17 @@
         <v>0.15</v>
       </c>
       <c r="E8" s="1">
-        <v>-8</v>
+        <v>-5</v>
       </c>
       <c r="F8" s="1">
-        <v>-10</v>
+        <v>-7</v>
       </c>
       <c r="M8" s="1">
         <v>800</v>
       </c>
       <c r="N8" s="1">
         <f t="shared" si="0"/>
-        <v>30.4</v>
+        <v>26.2</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
@@ -1469,20 +1469,20 @@
         <v>10</v>
       </c>
       <c r="D9" s="1">
-        <v>0.4</v>
+        <v>0.41</v>
       </c>
       <c r="E9" s="1">
-        <v>-16</v>
+        <v>-12</v>
       </c>
       <c r="F9" s="1">
-        <v>-21</v>
+        <v>-17</v>
       </c>
       <c r="M9" s="1">
         <v>700</v>
       </c>
       <c r="N9" s="1">
         <f t="shared" si="0"/>
-        <v>27.4</v>
+        <v>21.6</v>
       </c>
       <c r="P9" s="1">
         <v>25</v>
@@ -1649,17 +1649,17 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="E15" s="1">
-        <v>-17</v>
+        <v>-14</v>
       </c>
       <c r="F15" s="1">
-        <v>-8</v>
+        <v>-5</v>
       </c>
       <c r="M15" s="1">
         <v>700</v>
       </c>
       <c r="N15" s="1">
         <f t="shared" si="0"/>
-        <v>26.6</v>
+        <v>22.4</v>
       </c>
       <c r="P15" s="1">
         <v>21.3</v>
@@ -1682,10 +1682,10 @@
         <v>0.15</v>
       </c>
       <c r="E16" s="1">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="F16" s="1">
-        <v>-3</v>
+        <v>-1</v>
       </c>
       <c r="H16" s="1">
         <v>-0.4</v>
@@ -1695,7 +1695,7 @@
       </c>
       <c r="N16" s="1">
         <f t="shared" si="0"/>
-        <v>-0.60000000000000053</v>
+        <v>-2.6000000000000005</v>
       </c>
       <c r="R16" s="1">
         <v>95</v>
@@ -1715,17 +1715,17 @@
         <v>0.38</v>
       </c>
       <c r="E17" s="1">
-        <v>-3</v>
+        <v>-2</v>
       </c>
       <c r="F17" s="1">
-        <v>-8</v>
+        <v>-4</v>
       </c>
       <c r="M17" s="1">
         <v>1200</v>
       </c>
       <c r="N17" s="1">
         <f t="shared" si="0"/>
-        <v>22.6</v>
+        <v>19.399999999999999</v>
       </c>
       <c r="P17" s="1">
         <v>31.4</v>
@@ -1748,17 +1748,17 @@
         <v>0.16</v>
       </c>
       <c r="E18" s="1">
-        <v>-9</v>
+        <v>-7</v>
       </c>
       <c r="F18" s="1">
-        <v>-11</v>
+        <v>-8</v>
       </c>
       <c r="M18" s="1">
         <v>1000</v>
       </c>
       <c r="N18" s="1">
         <f t="shared" si="0"/>
-        <v>25.6</v>
+        <v>22.200000000000003</v>
       </c>
       <c r="P18" s="1">
         <v>15.2</v>
@@ -1811,17 +1811,17 @@
         <v>0.32</v>
       </c>
       <c r="E21" s="1">
-        <v>-13</v>
+        <v>-9</v>
       </c>
       <c r="F21" s="1">
-        <v>-13</v>
+        <v>-9</v>
       </c>
       <c r="M21" s="1">
         <v>1000</v>
       </c>
       <c r="N21" s="1">
         <f t="shared" si="0"/>
-        <v>25.8</v>
+        <v>20.2</v>
       </c>
       <c r="P21" s="1">
         <v>19</v>
@@ -1871,17 +1871,17 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="E23" s="1">
-        <v>-4</v>
+        <v>-2</v>
       </c>
       <c r="F23" s="1">
-        <v>-5</v>
+        <v>-3</v>
       </c>
       <c r="M23" s="1">
         <v>500</v>
       </c>
       <c r="N23" s="1">
         <f t="shared" si="0"/>
-        <v>19.599999999999998</v>
+        <v>16.799999999999997</v>
       </c>
       <c r="P23" s="1">
         <v>14.4</v>
@@ -1901,10 +1901,10 @@
         <v>0.12</v>
       </c>
       <c r="E24" s="1">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="F24" s="1">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="H24" s="1">
         <v>0</v>
@@ -1914,7 +1914,7 @@
       </c>
       <c r="N24" s="1">
         <f t="shared" si="0"/>
-        <v>-0.59999999999999987</v>
+        <v>-1.9999999999999996</v>
       </c>
       <c r="P24" s="1">
         <v>3.8</v>
@@ -1937,10 +1937,10 @@
         <v>0.15</v>
       </c>
       <c r="E25" s="1">
+        <v>-1</v>
+      </c>
+      <c r="F25" s="1">
         <v>-2</v>
-      </c>
-      <c r="F25" s="1">
-        <v>-3</v>
       </c>
       <c r="H25" s="1">
         <v>-0.1</v>
@@ -1950,7 +1950,7 @@
       </c>
       <c r="N25" s="1">
         <f t="shared" si="0"/>
-        <v>-1.1000000000000001</v>
+        <v>-2.5</v>
       </c>
       <c r="P25" s="1">
         <v>6</v>
@@ -1976,17 +1976,17 @@
         <v>0.2</v>
       </c>
       <c r="E27" s="1">
-        <v>-16</v>
+        <v>-12</v>
       </c>
       <c r="F27" s="1">
-        <v>-7</v>
+        <v>-6</v>
       </c>
       <c r="M27" s="1">
         <v>900</v>
       </c>
       <c r="N27" s="1">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>26.200000000000003</v>
       </c>
       <c r="P27" s="1">
         <v>15.8</v>
@@ -2009,17 +2009,17 @@
         <v>0.25</v>
       </c>
       <c r="E28" s="1">
-        <v>-6</v>
+        <v>-5</v>
       </c>
       <c r="F28" s="1">
-        <v>-24</v>
+        <v>-19</v>
       </c>
       <c r="M28" s="1">
         <v>1000</v>
       </c>
       <c r="N28" s="1">
         <f t="shared" si="0"/>
-        <v>30.2</v>
+        <v>26.4</v>
       </c>
       <c r="P28" s="1">
         <v>13</v>
@@ -2042,17 +2042,17 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="E29" s="1">
-        <v>-8</v>
+        <v>-6</v>
       </c>
       <c r="F29" s="1">
-        <v>-10</v>
+        <v>-7</v>
       </c>
       <c r="M29" s="1">
         <v>500</v>
       </c>
       <c r="N29" s="1">
         <f t="shared" si="0"/>
-        <v>27.6</v>
+        <v>24.2</v>
       </c>
       <c r="P29" s="1">
         <v>6.6</v>
@@ -2102,17 +2102,17 @@
         <v>0.19</v>
       </c>
       <c r="E31" s="1">
-        <v>-12</v>
+        <v>-9</v>
       </c>
       <c r="F31" s="1">
-        <v>-11</v>
+        <v>-8</v>
       </c>
       <c r="M31" s="1">
         <v>800</v>
       </c>
       <c r="N31" s="1">
         <f t="shared" si="0"/>
-        <v>29.4</v>
+        <v>25.2</v>
       </c>
       <c r="P31" s="1">
         <v>8.4</v>
@@ -2162,17 +2162,17 @@
         <v>0.22</v>
       </c>
       <c r="E33" s="1">
-        <v>-10</v>
+        <v>-7</v>
       </c>
       <c r="F33" s="1">
-        <v>-15</v>
+        <v>-12</v>
       </c>
       <c r="M33" s="1">
         <v>800</v>
       </c>
       <c r="N33" s="1">
         <f t="shared" si="0"/>
-        <v>28.6</v>
+        <v>24.4</v>
       </c>
       <c r="P33" s="1">
         <v>15.5</v>
@@ -2222,17 +2222,17 @@
         <v>0.26</v>
       </c>
       <c r="E35" s="1">
-        <v>-14</v>
+        <v>-11</v>
       </c>
       <c r="F35" s="1">
-        <v>-14</v>
+        <v>-11</v>
       </c>
       <c r="M35" s="1">
         <v>700</v>
       </c>
       <c r="N35" s="1">
         <f t="shared" si="0"/>
-        <v>28.4</v>
+        <v>24.200000000000003</v>
       </c>
       <c r="P35" s="1">
         <v>14</v>
@@ -2282,17 +2282,17 @@
         <v>0.35</v>
       </c>
       <c r="E37" s="1">
-        <v>-6</v>
+        <v>-5</v>
       </c>
       <c r="F37" s="1">
-        <v>-5</v>
+        <v>-3</v>
       </c>
       <c r="M37" s="1">
         <v>1500</v>
       </c>
       <c r="N37" s="1">
         <f t="shared" si="0"/>
-        <v>20.8</v>
+        <v>18.8</v>
       </c>
       <c r="P37" s="1">
         <v>27.8</v>
@@ -2330,7 +2330,7 @@
         <v>66</v>
       </c>
       <c r="C39" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D39" s="1">
         <v>0.04</v>
@@ -2346,7 +2346,7 @@
       </c>
       <c r="N39" s="1">
         <f t="shared" si="0"/>
-        <v>2.6</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">
@@ -2363,17 +2363,17 @@
         <v>0.21</v>
       </c>
       <c r="E40" s="1">
-        <v>-12</v>
+        <v>-9</v>
       </c>
       <c r="F40" s="1">
-        <v>-16</v>
+        <v>-13</v>
       </c>
       <c r="M40" s="1">
         <v>600</v>
       </c>
       <c r="N40" s="1">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>25.8</v>
       </c>
       <c r="P40" s="1">
         <v>9.5</v>
@@ -2396,17 +2396,17 @@
         <v>0.22</v>
       </c>
       <c r="E41" s="1">
-        <v>-15</v>
+        <v>-12</v>
       </c>
       <c r="F41" s="1">
-        <v>-10</v>
+        <v>-7</v>
       </c>
       <c r="M41" s="1">
         <v>750</v>
       </c>
       <c r="N41" s="1">
         <f t="shared" si="0"/>
-        <v>29.6</v>
+        <v>25.400000000000002</v>
       </c>
       <c r="P41" s="1">
         <v>10</v>
@@ -2426,17 +2426,17 @@
         <v>0.2</v>
       </c>
       <c r="E42" s="1">
-        <v>-12</v>
+        <v>-8</v>
       </c>
       <c r="F42" s="1">
-        <v>-10</v>
+        <v>-6</v>
       </c>
       <c r="M42" s="1">
         <v>0</v>
       </c>
       <c r="N42" s="1">
         <f t="shared" si="0"/>
-        <v>27.6</v>
+        <v>22</v>
       </c>
       <c r="P42" s="1">
         <v>8</v>
@@ -2483,17 +2483,17 @@
         <v>0.24</v>
       </c>
       <c r="E44" s="1">
-        <v>-6</v>
+        <v>-4</v>
       </c>
       <c r="F44" s="1">
-        <v>-18</v>
+        <v>-14</v>
       </c>
       <c r="M44" s="1">
         <v>700</v>
       </c>
       <c r="N44" s="1">
         <f t="shared" si="0"/>
-        <v>28.799999999999997</v>
+        <v>24.799999999999997</v>
       </c>
       <c r="P44" s="1">
         <v>12.4</v>
@@ -2516,17 +2516,17 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="E45" s="1">
-        <v>-9</v>
+        <v>-6</v>
       </c>
       <c r="F45" s="1">
-        <v>-14</v>
+        <v>-11</v>
       </c>
       <c r="M45" s="1">
         <v>500</v>
       </c>
       <c r="N45" s="1">
         <f t="shared" si="0"/>
-        <v>27.799999999999997</v>
+        <v>23.6</v>
       </c>
       <c r="P45" s="1">
         <v>4.5999999999999996</v>
@@ -2579,17 +2579,17 @@
         <v>0.23</v>
       </c>
       <c r="E47" s="1">
-        <v>-12</v>
+        <v>-9</v>
       </c>
       <c r="F47" s="1">
-        <v>-12</v>
+        <v>-9</v>
       </c>
       <c r="M47" s="1">
         <v>900</v>
       </c>
       <c r="N47" s="1">
         <f t="shared" si="0"/>
-        <v>29.2</v>
+        <v>24.999999999999996</v>
       </c>
       <c r="P47" s="1">
         <v>12.6</v>
@@ -2639,17 +2639,17 @@
         <v>0.17</v>
       </c>
       <c r="E49" s="1">
-        <v>-10</v>
+        <v>-7</v>
       </c>
       <c r="F49" s="1">
-        <v>-11</v>
+        <v>-8</v>
       </c>
       <c r="M49" s="1">
         <v>800</v>
       </c>
       <c r="N49" s="1">
         <f t="shared" si="0"/>
-        <v>29.200000000000003</v>
+        <v>25</v>
       </c>
       <c r="P49" s="1">
         <v>7.8</v>
@@ -2699,17 +2699,17 @@
         <v>0.18</v>
       </c>
       <c r="E51" s="1">
-        <v>-11</v>
+        <v>-8</v>
       </c>
       <c r="F51" s="1">
-        <v>-13</v>
+        <v>-10</v>
       </c>
       <c r="M51" s="1">
         <v>900</v>
       </c>
       <c r="N51" s="1">
         <f t="shared" si="0"/>
-        <v>29.000000000000004</v>
+        <v>24.8</v>
       </c>
       <c r="P51" s="1">
         <v>8</v>
@@ -2768,11 +2768,11 @@
       </c>
       <c r="E55" s="1">
         <f t="shared" si="1"/>
-        <v>-10</v>
+        <v>-8</v>
       </c>
       <c r="F55" s="1">
         <f t="shared" si="1"/>
-        <v>-14</v>
+        <v>-12</v>
       </c>
       <c r="G55" s="1">
         <f t="shared" si="1"/>
@@ -2804,7 +2804,7 @@
       </c>
       <c r="N55" s="1">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>17.2</v>
       </c>
       <c r="P55" s="1">
         <f>P4+P3</f>
@@ -2837,11 +2837,11 @@
       </c>
       <c r="E56" s="1">
         <f t="shared" si="3"/>
-        <v>-8</v>
+        <v>-5</v>
       </c>
       <c r="F56" s="1">
         <f t="shared" si="3"/>
-        <v>-10</v>
+        <v>-7</v>
       </c>
       <c r="G56" s="1">
         <f t="shared" si="3"/>
@@ -2873,7 +2873,7 @@
       </c>
       <c r="N56" s="1">
         <f t="shared" si="0"/>
-        <v>25.799999999999997</v>
+        <v>21.599999999999998</v>
       </c>
       <c r="P56" s="1">
         <f>P8+P7+P5</f>
@@ -2902,15 +2902,15 @@
       </c>
       <c r="D57" s="1">
         <f t="shared" si="5"/>
-        <v>0.41000000000000003</v>
+        <v>0.42</v>
       </c>
       <c r="E57" s="1">
         <f t="shared" si="5"/>
-        <v>-16</v>
+        <v>-12</v>
       </c>
       <c r="F57" s="1">
         <f t="shared" si="5"/>
-        <v>-21</v>
+        <v>-17</v>
       </c>
       <c r="G57" s="1">
         <f t="shared" si="5"/>
@@ -2942,7 +2942,7 @@
       </c>
       <c r="N57" s="1">
         <f t="shared" si="0"/>
-        <v>27.2</v>
+        <v>21.4</v>
       </c>
       <c r="P57" s="1">
         <f>P9+P5</f>
@@ -3113,11 +3113,11 @@
       </c>
       <c r="E60" s="1">
         <f t="shared" si="8"/>
-        <v>-18</v>
+        <v>-15</v>
       </c>
       <c r="F60" s="1">
         <f t="shared" si="8"/>
-        <v>-10</v>
+        <v>-7</v>
       </c>
       <c r="G60" s="1">
         <f t="shared" si="8"/>
@@ -3149,7 +3149,7 @@
       </c>
       <c r="N60" s="1">
         <f t="shared" si="0"/>
-        <v>25.6</v>
+        <v>21.4</v>
       </c>
       <c r="P60" s="1">
         <f>P15+P14+P5</f>
@@ -3182,11 +3182,11 @@
       </c>
       <c r="E61" s="1">
         <f t="shared" si="9"/>
-        <v>-5</v>
+        <v>-3</v>
       </c>
       <c r="F61" s="1">
         <f t="shared" si="9"/>
-        <v>-11</v>
+        <v>-5</v>
       </c>
       <c r="G61" s="1">
         <f t="shared" si="9"/>
@@ -3218,7 +3218,7 @@
       </c>
       <c r="N61" s="1">
         <f t="shared" si="0"/>
-        <v>21.799999999999997</v>
+        <v>16.600000000000001</v>
       </c>
       <c r="P61" s="1">
         <f>P17+P16+P5</f>
@@ -3251,11 +3251,11 @@
       </c>
       <c r="E62" s="1">
         <f t="shared" si="10"/>
-        <v>-11</v>
+        <v>-8</v>
       </c>
       <c r="F62" s="1">
         <f t="shared" si="10"/>
-        <v>-14</v>
+        <v>-9</v>
       </c>
       <c r="G62" s="1">
         <f t="shared" si="10"/>
@@ -3287,7 +3287,7 @@
       </c>
       <c r="N62" s="1">
         <f t="shared" si="0"/>
-        <v>24.8</v>
+        <v>19.399999999999999</v>
       </c>
       <c r="P62" s="1">
         <f>P18+P16+P5</f>
@@ -3320,11 +3320,11 @@
       </c>
       <c r="E63" s="1">
         <f t="shared" si="11"/>
-        <v>-14</v>
+        <v>-10</v>
       </c>
       <c r="F63" s="1">
         <f t="shared" si="11"/>
-        <v>-14</v>
+        <v>-10</v>
       </c>
       <c r="G63" s="1">
         <f t="shared" si="11"/>
@@ -3356,7 +3356,7 @@
       </c>
       <c r="N63" s="1">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>22.4</v>
       </c>
       <c r="P63" s="1">
         <f>P22+P21+P19+P5</f>
@@ -3389,11 +3389,11 @@
       </c>
       <c r="E64" s="1">
         <f t="shared" si="12"/>
-        <v>-4</v>
+        <v>-2</v>
       </c>
       <c r="F64" s="1">
         <f t="shared" si="12"/>
-        <v>-5</v>
+        <v>-3</v>
       </c>
       <c r="G64" s="1">
         <f t="shared" si="12"/>
@@ -3425,7 +3425,7 @@
       </c>
       <c r="N64" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>16.2</v>
       </c>
       <c r="P64" s="1">
         <f>P23+P19+P5</f>
@@ -3458,11 +3458,11 @@
       </c>
       <c r="E65" s="1">
         <f t="shared" si="13"/>
-        <v>-18</v>
+        <v>-13</v>
       </c>
       <c r="F65" s="1">
         <f t="shared" si="13"/>
-        <v>-9</v>
+        <v>-7</v>
       </c>
       <c r="G65" s="1">
         <f t="shared" si="13"/>
@@ -3494,7 +3494,7 @@
       </c>
       <c r="N65" s="1">
         <f t="shared" si="0"/>
-        <v>28.799999999999997</v>
+        <v>23.599999999999998</v>
       </c>
       <c r="P65" s="1">
         <f>P27+P24+P19+P5</f>
@@ -3527,11 +3527,11 @@
       </c>
       <c r="E66" s="1">
         <f t="shared" si="14"/>
-        <v>-8</v>
+        <v>-6</v>
       </c>
       <c r="F66" s="1">
         <f t="shared" si="14"/>
-        <v>-26</v>
+        <v>-20</v>
       </c>
       <c r="G66" s="1">
         <f t="shared" si="14"/>
@@ -3563,7 +3563,7 @@
       </c>
       <c r="N66" s="1">
         <f t="shared" si="0"/>
-        <v>29</v>
+        <v>23.8</v>
       </c>
       <c r="P66" s="1">
         <f>P28+P24+P19+P5</f>
@@ -3596,11 +3596,11 @@
       </c>
       <c r="E67" s="1">
         <f t="shared" si="15"/>
-        <v>-11</v>
+        <v>-8</v>
       </c>
       <c r="F67" s="1">
         <f t="shared" si="15"/>
-        <v>-13</v>
+        <v>-9</v>
       </c>
       <c r="G67" s="1">
         <f t="shared" si="15"/>
@@ -3632,7 +3632,7 @@
       </c>
       <c r="N67" s="1">
         <f t="shared" si="0"/>
-        <v>28.400000000000002</v>
+        <v>23.599999999999998</v>
       </c>
       <c r="P67" s="1">
         <f>P29+P30+P24+P19+P5</f>
@@ -3665,11 +3665,11 @@
       </c>
       <c r="E68" s="1">
         <f t="shared" si="16"/>
-        <v>-15</v>
+        <v>-11</v>
       </c>
       <c r="F68" s="1">
         <f t="shared" si="16"/>
-        <v>-14</v>
+        <v>-10</v>
       </c>
       <c r="G68" s="1">
         <f t="shared" si="16"/>
@@ -3701,7 +3701,7 @@
       </c>
       <c r="N68" s="1">
         <f t="shared" si="0"/>
-        <v>30.200000000000003</v>
+        <v>24.6</v>
       </c>
       <c r="P68" s="1">
         <f>P32+P31+P24+P19+P5</f>
@@ -3734,11 +3734,11 @@
       </c>
       <c r="E69" s="1">
         <f t="shared" si="17"/>
-        <v>-13</v>
+        <v>-9</v>
       </c>
       <c r="F69" s="1">
         <f t="shared" si="17"/>
-        <v>-18</v>
+        <v>-14</v>
       </c>
       <c r="G69" s="1">
         <f t="shared" si="17"/>
@@ -3770,7 +3770,7 @@
       </c>
       <c r="N69" s="1">
         <f t="shared" si="0"/>
-        <v>29.199999999999996</v>
+        <v>23.6</v>
       </c>
       <c r="P69" s="1">
         <f>P34+P33+P24+P19+P5</f>
@@ -3803,11 +3803,11 @@
       </c>
       <c r="E70" s="1">
         <f t="shared" si="18"/>
-        <v>-17</v>
+        <v>-13</v>
       </c>
       <c r="F70" s="1">
         <f t="shared" si="18"/>
-        <v>-17</v>
+        <v>-13</v>
       </c>
       <c r="G70" s="1">
         <f t="shared" si="18"/>
@@ -3839,7 +3839,7 @@
       </c>
       <c r="N70" s="1">
         <f t="shared" si="0"/>
-        <v>29.099999999999998</v>
+        <v>23.5</v>
       </c>
       <c r="P70" s="1">
         <f>P36+P35+P24+P19+P5</f>
@@ -3864,7 +3864,7 @@
       </c>
       <c r="C71" s="1">
         <f t="shared" ref="C71:M71" si="19">C39+C38+C37+C24+C19+C5</f>
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D71" s="1">
         <f t="shared" si="19"/>
@@ -3872,11 +3872,11 @@
       </c>
       <c r="E71" s="1">
         <f t="shared" si="19"/>
-        <v>-9</v>
+        <v>-7</v>
       </c>
       <c r="F71" s="1">
         <f t="shared" si="19"/>
-        <v>-8</v>
+        <v>-5</v>
       </c>
       <c r="G71" s="1">
         <f t="shared" si="19"/>
@@ -3908,7 +3908,7 @@
       </c>
       <c r="N71" s="1">
         <f t="shared" ref="N71:N77" si="20">C71-(D71*20)-(E71*0.8)-(F71*0.6)-(H71*5)</f>
-        <v>21.200000000000003</v>
+        <v>16.8</v>
       </c>
       <c r="P71" s="1">
         <f>P39+P38+P37+P24+P19+P5</f>
@@ -3941,11 +3941,11 @@
       </c>
       <c r="E72" s="1">
         <f t="shared" si="21"/>
-        <v>-14</v>
+        <v>-10</v>
       </c>
       <c r="F72" s="1">
         <f t="shared" si="21"/>
-        <v>-18</v>
+        <v>-14</v>
       </c>
       <c r="G72" s="1">
         <f t="shared" si="21"/>
@@ -3977,7 +3977,7 @@
       </c>
       <c r="N72" s="1">
         <f t="shared" si="20"/>
-        <v>28.799999999999997</v>
+        <v>23.200000000000003</v>
       </c>
       <c r="P72" s="1">
         <f>P40+P24+P19+P5</f>
@@ -4010,11 +4010,11 @@
       </c>
       <c r="E73" s="1">
         <f t="shared" si="22"/>
-        <v>-17</v>
+        <v>-13</v>
       </c>
       <c r="F73" s="1">
         <f t="shared" si="22"/>
-        <v>-12</v>
+        <v>-8</v>
       </c>
       <c r="G73" s="1">
         <f t="shared" si="22"/>
@@ -4046,7 +4046,7 @@
       </c>
       <c r="N73" s="1">
         <f t="shared" si="20"/>
-        <v>28.400000000000002</v>
+        <v>22.8</v>
       </c>
       <c r="P73" s="1">
         <f>P41+P24+P19+P5</f>
@@ -4079,11 +4079,11 @@
       </c>
       <c r="E74" s="1">
         <f t="shared" si="23"/>
-        <v>-14</v>
+        <v>-9</v>
       </c>
       <c r="F74" s="1">
         <f t="shared" si="23"/>
-        <v>-12</v>
+        <v>-7</v>
       </c>
       <c r="G74" s="1">
         <f t="shared" si="23"/>
@@ -4115,7 +4115,7 @@
       </c>
       <c r="N74" s="1">
         <f t="shared" si="20"/>
-        <v>26.4</v>
+        <v>19.399999999999999</v>
       </c>
       <c r="P74" s="1">
         <f>P42+P24+P19+P5</f>
@@ -4148,11 +4148,11 @@
       </c>
       <c r="E75" s="1">
         <f t="shared" si="24"/>
-        <v>-9</v>
+        <v>-6</v>
       </c>
       <c r="F75" s="1">
         <f t="shared" si="24"/>
-        <v>-21</v>
+        <v>-16</v>
       </c>
       <c r="G75" s="1">
         <f t="shared" si="24"/>
@@ -4184,7 +4184,7 @@
       </c>
       <c r="N75" s="1">
         <f t="shared" si="20"/>
-        <v>29.6</v>
+        <v>24.2</v>
       </c>
       <c r="P75" s="1">
         <f>P44+P43+P24+P19+P5</f>
@@ -4217,11 +4217,11 @@
       </c>
       <c r="E76" s="1">
         <f t="shared" si="25"/>
-        <v>-12</v>
+        <v>-8</v>
       </c>
       <c r="F76" s="1">
         <f t="shared" si="25"/>
-        <v>-17</v>
+        <v>-13</v>
       </c>
       <c r="G76" s="1">
         <f t="shared" si="25"/>
@@ -4253,7 +4253,7 @@
       </c>
       <c r="N76" s="1">
         <f t="shared" si="20"/>
-        <v>29.2</v>
+        <v>23.599999999999998</v>
       </c>
       <c r="P76" s="1">
         <f>P46+P45+P24+P19+P5</f>
@@ -4286,11 +4286,11 @@
       </c>
       <c r="E77" s="1">
         <f t="shared" si="26"/>
-        <v>-15</v>
+        <v>-11</v>
       </c>
       <c r="F77" s="1">
         <f t="shared" si="26"/>
-        <v>-15</v>
+        <v>-11</v>
       </c>
       <c r="G77" s="1">
         <f t="shared" si="26"/>
@@ -4322,7 +4322,7 @@
       </c>
       <c r="N77" s="1">
         <f t="shared" si="20"/>
-        <v>30</v>
+        <v>24.4</v>
       </c>
       <c r="P77" s="1">
         <f>P48+P47+P24+P19+P5</f>
@@ -4355,11 +4355,11 @@
       </c>
       <c r="E78" s="1">
         <f t="shared" si="27"/>
-        <v>-13</v>
+        <v>-9</v>
       </c>
       <c r="F78" s="1">
         <f t="shared" si="27"/>
-        <v>-14</v>
+        <v>-10</v>
       </c>
       <c r="G78" s="1">
         <f t="shared" si="27"/>
@@ -4391,7 +4391,7 @@
       </c>
       <c r="N78" s="1">
         <f t="shared" si="28"/>
-        <v>30.000000000000004</v>
+        <v>24.400000000000002</v>
       </c>
       <c r="P78" s="1">
         <f t="shared" si="28"/>
@@ -4424,11 +4424,11 @@
       </c>
       <c r="E79" s="1">
         <f t="shared" si="29"/>
-        <v>-14</v>
+        <v>-10</v>
       </c>
       <c r="F79" s="1">
         <f t="shared" si="29"/>
-        <v>-16</v>
+        <v>-12</v>
       </c>
       <c r="G79" s="1">
         <f t="shared" si="29"/>
@@ -4460,7 +4460,7 @@
       </c>
       <c r="N79" s="1">
         <f t="shared" si="29"/>
-        <v>29.800000000000004</v>
+        <v>24.200000000000003</v>
       </c>
       <c r="P79" s="1">
         <f t="shared" si="29"/>

</xml_diff>

<commit_message>
kill vector brace more
</commit_message>
<xml_diff>
--- a/changes/m4-stocks.xlsx
+++ b/changes/m4-stocks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lingl\Documents\deadline-balancing\changes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B7B0B7AE-6C63-41AE-AA5A-5618BA0132ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19DC9D95-B72B-4086-B79C-92B0656B9426}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1239,8 +1239,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S79"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M52" sqref="M52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1709,13 +1709,13 @@
         <v>32</v>
       </c>
       <c r="C17" s="1">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D17" s="1">
         <v>0.38</v>
       </c>
       <c r="E17" s="1">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="F17" s="1">
         <v>-4</v>
@@ -1725,7 +1725,7 @@
       </c>
       <c r="N17" s="1">
         <f t="shared" si="0"/>
-        <v>19.399999999999999</v>
+        <v>19.2</v>
       </c>
       <c r="P17" s="1">
         <v>31.4</v>
@@ -1865,13 +1865,13 @@
         <v>41</v>
       </c>
       <c r="C23" s="1">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D23" s="1">
         <v>0.28000000000000003</v>
       </c>
       <c r="E23" s="1">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="F23" s="1">
         <v>-3</v>
@@ -1881,7 +1881,7 @@
       </c>
       <c r="N23" s="1">
         <f t="shared" si="0"/>
-        <v>16.799999999999997</v>
+        <v>16.599999999999998</v>
       </c>
       <c r="P23" s="1">
         <v>14.4</v>
@@ -2282,7 +2282,7 @@
         <v>0.35</v>
       </c>
       <c r="E37" s="1">
-        <v>-5</v>
+        <v>-4</v>
       </c>
       <c r="F37" s="1">
         <v>-3</v>
@@ -2292,7 +2292,7 @@
       </c>
       <c r="N37" s="1">
         <f t="shared" si="0"/>
-        <v>18.8</v>
+        <v>18</v>
       </c>
       <c r="P37" s="1">
         <v>27.8</v>
@@ -2966,20 +2966,20 @@
         <v>23</v>
       </c>
       <c r="C58" s="1">
-        <f t="shared" ref="C58:M58" si="6">C11+C10+C5</f>
-        <v>21</v>
+        <f>C11+C10+C5+C13</f>
+        <v>23</v>
       </c>
       <c r="D58" s="1">
-        <f t="shared" si="6"/>
-        <v>0.35</v>
+        <f>D11+D10+D5+D13</f>
+        <v>0.39999999999999997</v>
       </c>
       <c r="E58" s="1">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f t="shared" ref="E58:M58" si="6">E11+E10+E5+E13</f>
+        <v>-1</v>
       </c>
       <c r="F58" s="1">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="G58" s="1">
         <f t="shared" si="6"/>
@@ -3011,7 +3011,7 @@
       </c>
       <c r="N58" s="1">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>16.400000000000002</v>
       </c>
       <c r="P58" s="1">
         <f>P11+P10+P5</f>
@@ -3035,20 +3035,20 @@
         <v>25</v>
       </c>
       <c r="C59" s="1">
-        <f t="shared" ref="C59:M59" si="7">C12+C10+C5</f>
-        <v>21</v>
+        <f>C12+C10+C5+C13</f>
+        <v>23</v>
       </c>
       <c r="D59" s="1">
-        <f t="shared" si="7"/>
-        <v>0.33</v>
+        <f t="shared" ref="D59:M59" si="7">D12+D10+D5+D13</f>
+        <v>0.38</v>
       </c>
       <c r="E59" s="1">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F59" s="1">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="G59" s="1">
         <f t="shared" si="7"/>
@@ -3080,7 +3080,7 @@
       </c>
       <c r="N59" s="1">
         <f t="shared" si="0"/>
-        <v>14.399999999999999</v>
+        <v>16.8</v>
       </c>
       <c r="P59" s="1">
         <f>P12+P10+P5</f>
@@ -3174,7 +3174,7 @@
       </c>
       <c r="C61" s="1">
         <f t="shared" ref="C61:M61" si="9">C17+C16+C5</f>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D61" s="1">
         <f t="shared" si="9"/>
@@ -3182,7 +3182,7 @@
       </c>
       <c r="E61" s="1">
         <f t="shared" si="9"/>
-        <v>-3</v>
+        <v>-4</v>
       </c>
       <c r="F61" s="1">
         <f t="shared" si="9"/>
@@ -3218,7 +3218,7 @@
       </c>
       <c r="N61" s="1">
         <f t="shared" si="0"/>
-        <v>16.600000000000001</v>
+        <v>16.399999999999999</v>
       </c>
       <c r="P61" s="1">
         <f>P17+P16+P5</f>
@@ -3381,7 +3381,7 @@
       </c>
       <c r="C64" s="1">
         <f t="shared" ref="C64:M64" si="12">C23+C19+C5</f>
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D64" s="1">
         <f t="shared" si="12"/>
@@ -3389,7 +3389,7 @@
       </c>
       <c r="E64" s="1">
         <f t="shared" si="12"/>
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="F64" s="1">
         <f t="shared" si="12"/>
@@ -3425,7 +3425,7 @@
       </c>
       <c r="N64" s="1">
         <f t="shared" si="0"/>
-        <v>16.2</v>
+        <v>16</v>
       </c>
       <c r="P64" s="1">
         <f>P23+P19+P5</f>
@@ -3872,7 +3872,7 @@
       </c>
       <c r="E71" s="1">
         <f t="shared" si="19"/>
-        <v>-7</v>
+        <v>-6</v>
       </c>
       <c r="F71" s="1">
         <f t="shared" si="19"/>
@@ -3908,7 +3908,7 @@
       </c>
       <c r="N71" s="1">
         <f t="shared" ref="N71:N77" si="20">C71-(D71*20)-(E71*0.8)-(F71*0.6)-(H71*5)</f>
-        <v>16.8</v>
+        <v>16</v>
       </c>
       <c r="P71" s="1">
         <f>P39+P38+P37+P24+P19+P5</f>

</xml_diff>

<commit_message>
rename troy m7a1 and add new troy bcg
</commit_message>
<xml_diff>
--- a/changes/m4-stocks.xlsx
+++ b/changes/m4-stocks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yifan\Documents\deadline-balancing\changes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FC33055-C583-4325-A0C0-1D16E4456E16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77DA0FB5-9C0A-482C-933F-63AFEF6C558A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="126">
   <si>
     <t>name</t>
   </si>
@@ -74,18 +74,9 @@
     <t>Colt M4A1 Receiver Endplate</t>
   </si>
   <si>
-    <t>troy_m7a1</t>
-  </si>
-  <si>
     <t>Troy M7A1</t>
   </si>
   <si>
-    <t>ti_stock</t>
-  </si>
-  <si>
-    <t>Troy M7A1 Extendable Buttpad</t>
-  </si>
-  <si>
     <t>leapers_utg_model_15_fixed_a2_ar15_stock</t>
   </si>
   <si>
@@ -408,6 +399,18 @@
   </si>
   <si>
     <t>buck_barrel_deviation</t>
+  </si>
+  <si>
+    <t>troy_m7a1_pdw_extendable_stock</t>
+  </si>
+  <si>
+    <t>Troy M7A1 PDW Extendable Stock</t>
+  </si>
+  <si>
+    <t>troy_m7a1_pdw_base_stock</t>
+  </si>
+  <si>
+    <t>Troy M7A1 PDW Base</t>
   </si>
 </sst>
 </file>
@@ -1252,7 +1255,7 @@
   <dimension ref="A1:S82"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1264,7 +1267,7 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -1287,40 +1290,40 @@
         <v>5</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>85</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="N2" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="R2" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
@@ -1421,10 +1424,10 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C6" s="1">
         <v>-2</v>
@@ -1452,10 +1455,10 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C7" s="1">
         <v>16</v>
@@ -1482,58 +1485,58 @@
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C8" s="1">
+        <v>-2</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0.12</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0</v>
+      </c>
+      <c r="M8" s="1">
+        <v>1000</v>
+      </c>
       <c r="N8" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>C8-(D8*20)-(E8*0.8)-(F8*0.6)-(H8*5)</f>
+        <v>-4.4000000000000004</v>
+      </c>
+      <c r="P8" s="1">
+        <v>14</v>
       </c>
       <c r="Q8" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>P8*0.025</f>
+        <v>0.35000000000000003</v>
+      </c>
+      <c r="R8" s="1">
+        <v>479.99</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="1">
-        <v>-2</v>
-      </c>
-      <c r="D9" s="1">
-        <v>0.12</v>
-      </c>
-      <c r="E9" s="1">
-        <v>0</v>
-      </c>
-      <c r="F9" s="1">
-        <v>0</v>
-      </c>
-      <c r="M9" s="1">
-        <v>1000</v>
-      </c>
       <c r="N9" s="1">
         <f t="shared" si="0"/>
-        <v>-4.4000000000000004</v>
-      </c>
-      <c r="P9" s="1">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="Q9" s="1">
         <f t="shared" si="1"/>
-        <v>0.35000000000000003</v>
-      </c>
-      <c r="R9" s="1">
-        <v>479.99</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>15</v>
+        <v>122</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>16</v>
+        <v>123</v>
       </c>
       <c r="C10" s="1">
         <v>21</v>
@@ -1561,10 +1564,10 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C11" s="1">
         <v>11</v>
@@ -1598,10 +1601,10 @@
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C12" s="1">
         <v>-1</v>
@@ -1623,10 +1626,10 @@
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C13" s="1">
         <v>22</v>
@@ -1663,10 +1666,10 @@
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C14" s="1">
         <v>22</v>
@@ -1703,10 +1706,10 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C15" s="1">
         <v>1</v>
@@ -1734,10 +1737,10 @@
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C16" s="1">
         <v>-1</v>
@@ -1768,10 +1771,10 @@
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C17" s="1">
         <v>14</v>
@@ -1805,10 +1808,10 @@
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C18" s="1">
         <v>-2</v>
@@ -1842,10 +1845,10 @@
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C19" s="1">
         <v>22</v>
@@ -1879,10 +1882,10 @@
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C20" s="1">
         <v>15</v>
@@ -1916,10 +1919,10 @@
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C21" s="1">
         <v>0</v>
@@ -1954,10 +1957,10 @@
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C23" s="1">
         <v>14</v>
@@ -1991,10 +1994,10 @@
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C24" s="1">
         <v>2</v>
@@ -2022,10 +2025,10 @@
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C25" s="1">
         <v>18</v>
@@ -2056,10 +2059,10 @@
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C26" s="1">
         <v>-1</v>
@@ -2096,10 +2099,10 @@
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C27" s="1">
         <v>-2</v>
@@ -2143,10 +2146,10 @@
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C29" s="1">
         <v>17</v>
@@ -2180,10 +2183,10 @@
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C30" s="1">
         <v>16</v>
@@ -2217,10 +2220,10 @@
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C31" s="1">
         <v>18</v>
@@ -2254,10 +2257,10 @@
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C32" s="1">
         <v>1</v>
@@ -2285,10 +2288,10 @@
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C33" s="1">
         <v>17</v>
@@ -2322,10 +2325,10 @@
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C34" s="1">
         <v>1</v>
@@ -2353,10 +2356,10 @@
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C35" s="1">
         <v>16</v>
@@ -2390,10 +2393,10 @@
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C36" s="1">
         <v>1</v>
@@ -2421,10 +2424,10 @@
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C37" s="1">
         <v>14</v>
@@ -2458,10 +2461,10 @@
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C38" s="1">
         <v>1</v>
@@ -2489,10 +2492,10 @@
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C39" s="1">
         <v>20</v>
@@ -2529,10 +2532,10 @@
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C40" s="1">
         <v>0</v>
@@ -2554,10 +2557,10 @@
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C41" s="1">
         <v>1</v>
@@ -2585,10 +2588,10 @@
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C42" s="1">
         <v>15</v>
@@ -2622,10 +2625,10 @@
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C43" s="1">
         <v>16</v>
@@ -2656,10 +2659,10 @@
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C44" s="1">
         <v>16</v>
@@ -2690,10 +2693,10 @@
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C45" s="1">
         <v>1</v>
@@ -2721,10 +2724,10 @@
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C46" s="1">
         <v>18</v>
@@ -2758,10 +2761,10 @@
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C47" s="1">
         <v>16</v>
@@ -2795,10 +2798,10 @@
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C48" s="1">
         <v>1</v>
@@ -2829,10 +2832,10 @@
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C49" s="1">
         <v>17</v>
@@ -2866,10 +2869,10 @@
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C50" s="1">
         <v>1</v>
@@ -2897,10 +2900,10 @@
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C51" s="1">
         <v>18</v>
@@ -2934,10 +2937,10 @@
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C52" s="1">
         <v>1</v>
@@ -2965,10 +2968,10 @@
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C53" s="1">
         <v>16</v>
@@ -3002,10 +3005,10 @@
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C54" s="1">
         <v>1</v>
@@ -3039,7 +3042,7 @@
     </row>
     <row r="56" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B56" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="N56" s="1">
         <f t="shared" si="0"/>
@@ -3048,50 +3051,50 @@
     </row>
     <row r="57" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B57" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C57" s="1">
-        <f t="shared" ref="C57:P57" si="2">C4+C3</f>
+        <f>C4+C3</f>
         <v>11</v>
       </c>
       <c r="D57" s="1">
-        <f t="shared" si="2"/>
+        <f>D4+D3</f>
         <v>0.38</v>
       </c>
       <c r="E57" s="1">
-        <f t="shared" si="2"/>
+        <f>E4+E3</f>
         <v>-8</v>
       </c>
       <c r="F57" s="1">
-        <f t="shared" si="2"/>
+        <f>F4+F3</f>
         <v>-12</v>
       </c>
       <c r="G57" s="1">
-        <f t="shared" si="2"/>
+        <f>G4+G3</f>
         <v>0</v>
       </c>
       <c r="H57" s="1">
-        <f t="shared" si="2"/>
+        <f>H4+H3</f>
         <v>0</v>
       </c>
       <c r="I57" s="1">
-        <f t="shared" si="2"/>
+        <f>I4+I3</f>
         <v>0</v>
       </c>
       <c r="J57" s="1">
-        <f t="shared" si="2"/>
+        <f>J4+J3</f>
         <v>0</v>
       </c>
       <c r="K57" s="1">
-        <f t="shared" si="2"/>
+        <f>K4+K3</f>
         <v>0</v>
       </c>
       <c r="L57" s="1">
-        <f t="shared" si="2"/>
+        <f>L4+L3</f>
         <v>0</v>
       </c>
       <c r="M57" s="1">
-        <f t="shared" si="2"/>
+        <f>M4+M3</f>
         <v>1500</v>
       </c>
       <c r="N57" s="1">
@@ -3099,11 +3102,11 @@
         <v>17</v>
       </c>
       <c r="O57" s="1">
-        <f t="shared" si="2"/>
+        <f>O4+O3</f>
         <v>0</v>
       </c>
       <c r="P57" s="1">
-        <f t="shared" si="2"/>
+        <f>P4+P3</f>
         <v>19</v>
       </c>
       <c r="Q57" s="1">
@@ -3115,56 +3118,56 @@
         <v>129</v>
       </c>
       <c r="S57" s="1">
-        <f t="shared" ref="S57:S82" si="3">R57*3+500</f>
+        <f t="shared" ref="S57:S82" si="2">R57*3+500</f>
         <v>887</v>
       </c>
     </row>
     <row r="58" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B58" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C58" s="1">
         <f>C6+C7</f>
         <v>14</v>
       </c>
       <c r="D58" s="1">
-        <f t="shared" ref="D58:M58" si="4">D6+D7</f>
+        <f>D6+D7</f>
         <v>0.36</v>
       </c>
       <c r="E58" s="1">
-        <f t="shared" si="4"/>
+        <f>E6+E7</f>
         <v>-9</v>
       </c>
       <c r="F58" s="1">
-        <f t="shared" si="4"/>
+        <f>F6+F7</f>
         <v>-15</v>
       </c>
       <c r="G58" s="1">
-        <f t="shared" si="4"/>
+        <f>G6+G7</f>
         <v>0</v>
       </c>
       <c r="H58" s="1">
-        <f t="shared" si="4"/>
+        <f>H6+H7</f>
         <v>0</v>
       </c>
       <c r="I58" s="1">
-        <f t="shared" si="4"/>
+        <f>I6+I7</f>
         <v>0</v>
       </c>
       <c r="J58" s="1">
-        <f t="shared" si="4"/>
+        <f>J6+J7</f>
         <v>0</v>
       </c>
       <c r="K58" s="1">
-        <f t="shared" si="4"/>
+        <f>K6+K7</f>
         <v>0</v>
       </c>
       <c r="L58" s="1">
-        <f t="shared" si="4"/>
+        <f>L6+L7</f>
         <v>0</v>
       </c>
       <c r="M58" s="1">
-        <f t="shared" si="4"/>
+        <f>M6+M7</f>
         <v>1000</v>
       </c>
       <c r="N58" s="1">
@@ -3172,56 +3175,56 @@
         <v>23</v>
       </c>
       <c r="Q58" s="1">
-        <f t="shared" ref="Q58:Q82" si="5">P58*0.015+0.15</f>
+        <f t="shared" ref="Q58:Q82" si="3">P58*0.015+0.15</f>
         <v>0.15</v>
       </c>
     </row>
     <row r="59" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B59" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C59" s="1">
-        <f t="shared" ref="C59:M59" si="6">C10+C9+C5</f>
+        <f>C10+C8+C5</f>
         <v>19</v>
       </c>
       <c r="D59" s="1">
-        <f t="shared" si="6"/>
+        <f>D10+D8+D5</f>
         <v>0.28000000000000003</v>
       </c>
       <c r="E59" s="1">
-        <f t="shared" si="6"/>
+        <f>E10+E8+E5</f>
         <v>-6</v>
       </c>
       <c r="F59" s="1">
-        <f t="shared" si="6"/>
+        <f>F10+F8+F5</f>
         <v>-7</v>
       </c>
       <c r="G59" s="1">
-        <f t="shared" si="6"/>
+        <f>G10+G8+G5</f>
         <v>0</v>
       </c>
       <c r="H59" s="1">
-        <f t="shared" si="6"/>
+        <f>H10+H8+H5</f>
         <v>0</v>
       </c>
       <c r="I59" s="1">
-        <f t="shared" si="6"/>
+        <f>I10+I8+I5</f>
         <v>0</v>
       </c>
       <c r="J59" s="1">
-        <f t="shared" si="6"/>
+        <f>J10+J8+J5</f>
         <v>0</v>
       </c>
       <c r="K59" s="1">
-        <f t="shared" si="6"/>
+        <f>K10+K8+K5</f>
         <v>0</v>
       </c>
       <c r="L59" s="1">
-        <f t="shared" si="6"/>
+        <f>L10+L8+L5</f>
         <v>0</v>
       </c>
       <c r="M59" s="1">
-        <f t="shared" si="6"/>
+        <f>M10+M8+M5</f>
         <v>1800</v>
       </c>
       <c r="N59" s="1">
@@ -3229,68 +3232,68 @@
         <v>22.4</v>
       </c>
       <c r="P59" s="1">
-        <f>P10+P9+P5</f>
+        <f>P10+P8+P5</f>
         <v>14.4</v>
       </c>
       <c r="Q59" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>0.36599999999999999</v>
       </c>
       <c r="R59" s="1">
-        <f>R10+R9+R5</f>
+        <f>R10+R8+R5</f>
         <v>479.99</v>
       </c>
       <c r="S59" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1939.97</v>
       </c>
     </row>
     <row r="60" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B60" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C60" s="1">
-        <f t="shared" ref="C60:M60" si="7">C11+C5</f>
+        <f>C11+C5</f>
         <v>11</v>
       </c>
       <c r="D60" s="1">
-        <f t="shared" si="7"/>
+        <f>D11+D5</f>
         <v>0.45</v>
       </c>
       <c r="E60" s="1">
-        <f t="shared" si="7"/>
+        <f>E11+E5</f>
         <v>-12</v>
       </c>
       <c r="F60" s="1">
-        <f t="shared" si="7"/>
+        <f>F11+F5</f>
         <v>-18</v>
       </c>
       <c r="G60" s="1">
-        <f t="shared" si="7"/>
+        <f>G11+G5</f>
         <v>0</v>
       </c>
       <c r="H60" s="1">
-        <f t="shared" si="7"/>
+        <f>H11+H5</f>
         <v>0</v>
       </c>
       <c r="I60" s="1">
-        <f t="shared" si="7"/>
+        <f>I11+I5</f>
         <v>0</v>
       </c>
       <c r="J60" s="1">
-        <f t="shared" si="7"/>
+        <f>J11+J5</f>
         <v>0</v>
       </c>
       <c r="K60" s="1">
-        <f t="shared" si="7"/>
+        <f>K11+K5</f>
         <v>0</v>
       </c>
       <c r="L60" s="1">
-        <f t="shared" si="7"/>
+        <f>L11+L5</f>
         <v>0</v>
       </c>
       <c r="M60" s="1">
-        <f t="shared" si="7"/>
+        <f>M11+M5</f>
         <v>700</v>
       </c>
       <c r="N60" s="1">
@@ -3302,7 +3305,7 @@
         <v>25.4</v>
       </c>
       <c r="Q60" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>0.53099999999999992</v>
       </c>
       <c r="R60" s="1">
@@ -3310,13 +3313,13 @@
         <v>79.97</v>
       </c>
       <c r="S60" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>739.91</v>
       </c>
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B61" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C61" s="1">
         <f>C13+C12+C5+C15</f>
@@ -3327,39 +3330,39 @@
         <v>0.42</v>
       </c>
       <c r="E61" s="1">
-        <f t="shared" ref="E61:M61" si="8">E13+E12+E5+E15</f>
+        <f>E13+E12+E5+E15</f>
         <v>-1</v>
       </c>
       <c r="F61" s="1">
-        <f t="shared" si="8"/>
+        <f>F13+F12+F5+F15</f>
         <v>-1</v>
       </c>
       <c r="G61" s="1">
-        <f t="shared" si="8"/>
+        <f>G13+G12+G5+G15</f>
         <v>0</v>
       </c>
       <c r="H61" s="1">
-        <f t="shared" si="8"/>
+        <f>H13+H12+H5+H15</f>
         <v>-0.1</v>
       </c>
       <c r="I61" s="1">
-        <f t="shared" si="8"/>
+        <f>I13+I12+I5+I15</f>
         <v>0</v>
       </c>
       <c r="J61" s="1">
-        <f t="shared" si="8"/>
+        <f>J13+J12+J5+J15</f>
         <v>0</v>
       </c>
       <c r="K61" s="1">
-        <f t="shared" si="8"/>
+        <f>K13+K12+K5+K15</f>
         <v>0</v>
       </c>
       <c r="L61" s="1">
-        <f t="shared" si="8"/>
+        <f>L13+L12+L5+L15</f>
         <v>0</v>
       </c>
       <c r="M61" s="1">
-        <f t="shared" si="8"/>
+        <f>M13+M12+M5+M15</f>
         <v>1300</v>
       </c>
       <c r="N61" s="1">
@@ -3371,7 +3374,7 @@
         <v>32.08</v>
       </c>
       <c r="Q61" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>0.63119999999999998</v>
       </c>
       <c r="R61" s="1">
@@ -3379,56 +3382,56 @@
         <v>399.95</v>
       </c>
       <c r="S61" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1699.85</v>
       </c>
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B62" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C62" s="1">
         <f>C14+C12+C5+C15</f>
         <v>22</v>
       </c>
       <c r="D62" s="1">
-        <f t="shared" ref="D62:M62" si="9">D14+D12+D5+D15</f>
+        <f>D14+D12+D5+D15</f>
         <v>0.39999999999999997</v>
       </c>
       <c r="E62" s="1">
-        <f t="shared" si="9"/>
+        <f>E14+E12+E5+E15</f>
         <v>-1</v>
       </c>
       <c r="F62" s="1">
-        <f t="shared" si="9"/>
+        <f>F14+F12+F5+F15</f>
         <v>-1</v>
       </c>
       <c r="G62" s="1">
-        <f t="shared" si="9"/>
+        <f>G14+G12+G5+G15</f>
         <v>0</v>
       </c>
       <c r="H62" s="1">
-        <f t="shared" si="9"/>
+        <f>H14+H12+H5+H15</f>
         <v>-0.1</v>
       </c>
       <c r="I62" s="1">
-        <f t="shared" si="9"/>
+        <f>I14+I12+I5+I15</f>
         <v>0</v>
       </c>
       <c r="J62" s="1">
-        <f t="shared" si="9"/>
+        <f>J14+J12+J5+J15</f>
         <v>0</v>
       </c>
       <c r="K62" s="1">
-        <f t="shared" si="9"/>
+        <f>K14+K12+K5+K15</f>
         <v>0</v>
       </c>
       <c r="L62" s="1">
-        <f t="shared" si="9"/>
+        <f>L14+L12+L5+L15</f>
         <v>0</v>
       </c>
       <c r="M62" s="1">
-        <f t="shared" si="9"/>
+        <f>M14+M12+M5+M15</f>
         <v>1300</v>
       </c>
       <c r="N62" s="1">
@@ -3440,7 +3443,7 @@
         <v>32.08</v>
       </c>
       <c r="Q62" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>0.63119999999999998</v>
       </c>
       <c r="R62" s="1">
@@ -3448,56 +3451,56 @@
         <v>389.95</v>
       </c>
       <c r="S62" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1669.85</v>
       </c>
     </row>
     <row r="63" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B63" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C63" s="1">
-        <f t="shared" ref="C63:M63" si="10">C17+C16+C5</f>
+        <f>C17+C16+C5</f>
         <v>13</v>
       </c>
       <c r="D63" s="1">
-        <f t="shared" si="10"/>
+        <f>D17+D16+D5</f>
         <v>0.44</v>
       </c>
       <c r="E63" s="1">
-        <f t="shared" si="10"/>
+        <f>E17+E16+E5</f>
         <v>-15</v>
       </c>
       <c r="F63" s="1">
-        <f t="shared" si="10"/>
+        <f>F17+F16+F5</f>
         <v>-8</v>
       </c>
       <c r="G63" s="1">
-        <f t="shared" si="10"/>
+        <f>G17+G16+G5</f>
         <v>0</v>
       </c>
       <c r="H63" s="1">
-        <f t="shared" si="10"/>
+        <f>H17+H16+H5</f>
         <v>-0.1</v>
       </c>
       <c r="I63" s="1">
-        <f t="shared" si="10"/>
+        <f>I17+I16+I5</f>
         <v>0</v>
       </c>
       <c r="J63" s="1">
-        <f t="shared" si="10"/>
+        <f>J17+J16+J5</f>
         <v>0</v>
       </c>
       <c r="K63" s="1">
-        <f t="shared" si="10"/>
+        <f>K17+K16+K5</f>
         <v>0</v>
       </c>
       <c r="L63" s="1">
-        <f t="shared" si="10"/>
+        <f>L17+L16+L5</f>
         <v>0</v>
       </c>
       <c r="M63" s="1">
-        <f t="shared" si="10"/>
+        <f>M17+M16+M5</f>
         <v>1100</v>
       </c>
       <c r="N63" s="1">
@@ -3509,7 +3512,7 @@
         <v>21.7</v>
       </c>
       <c r="Q63" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>0.47549999999999992</v>
       </c>
       <c r="R63" s="1">
@@ -3517,56 +3520,56 @@
         <v>199.95</v>
       </c>
       <c r="S63" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1099.8499999999999</v>
       </c>
     </row>
     <row r="64" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B64" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C64" s="1">
-        <f t="shared" ref="C64:M64" si="11">C19+C18+C5</f>
+        <f>C19+C18+C5</f>
         <v>20</v>
       </c>
       <c r="D64" s="1">
-        <f t="shared" si="11"/>
+        <f>D19+D18+D5</f>
         <v>0.54</v>
       </c>
       <c r="E64" s="1">
-        <f t="shared" si="11"/>
+        <f>E19+E18+E5</f>
         <v>-4</v>
       </c>
       <c r="F64" s="1">
-        <f t="shared" si="11"/>
+        <f>F19+F18+F5</f>
         <v>-6</v>
       </c>
       <c r="G64" s="1">
-        <f t="shared" si="11"/>
+        <f>G19+G18+G5</f>
         <v>0</v>
       </c>
       <c r="H64" s="1">
-        <f t="shared" si="11"/>
+        <f>H19+H18+H5</f>
         <v>-0.1</v>
       </c>
       <c r="I64" s="1">
-        <f t="shared" si="11"/>
+        <f>I19+I18+I5</f>
         <v>0</v>
       </c>
       <c r="J64" s="1">
-        <f t="shared" si="11"/>
+        <f>J19+J18+J5</f>
         <v>0</v>
       </c>
       <c r="K64" s="1">
-        <f t="shared" si="11"/>
+        <f>K19+K18+K5</f>
         <v>0</v>
       </c>
       <c r="L64" s="1">
-        <f t="shared" si="11"/>
+        <f>L19+L18+L5</f>
         <v>0</v>
       </c>
       <c r="M64" s="1">
-        <f t="shared" si="11"/>
+        <f>M19+M18+M5</f>
         <v>1500</v>
       </c>
       <c r="N64" s="1">
@@ -3578,7 +3581,7 @@
         <v>31.799999999999997</v>
       </c>
       <c r="Q64" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>0.62699999999999989</v>
       </c>
       <c r="R64" s="1">
@@ -3586,56 +3589,56 @@
         <v>303.25</v>
       </c>
       <c r="S64" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1409.75</v>
       </c>
     </row>
     <row r="65" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B65" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C65" s="1">
-        <f t="shared" ref="C65:M65" si="12">C20+C18+C5</f>
+        <f>C20+C18+C5</f>
         <v>13</v>
       </c>
       <c r="D65" s="1">
-        <f t="shared" si="12"/>
+        <f>D20+D18+D5</f>
         <v>0.32</v>
       </c>
       <c r="E65" s="1">
-        <f t="shared" si="12"/>
+        <f>E20+E18+E5</f>
         <v>-8</v>
       </c>
       <c r="F65" s="1">
-        <f t="shared" si="12"/>
+        <f>F20+F18+F5</f>
         <v>-9</v>
       </c>
       <c r="G65" s="1">
-        <f t="shared" si="12"/>
+        <f>G20+G18+G5</f>
         <v>0</v>
       </c>
       <c r="H65" s="1">
-        <f t="shared" si="12"/>
+        <f>H20+H18+H5</f>
         <v>-0.1</v>
       </c>
       <c r="I65" s="1">
-        <f t="shared" si="12"/>
+        <f>I20+I18+I5</f>
         <v>0</v>
       </c>
       <c r="J65" s="1">
-        <f t="shared" si="12"/>
+        <f>J20+J18+J5</f>
         <v>0</v>
       </c>
       <c r="K65" s="1">
-        <f t="shared" si="12"/>
+        <f>K20+K18+K5</f>
         <v>0</v>
       </c>
       <c r="L65" s="1">
-        <f t="shared" si="12"/>
+        <f>L20+L18+L5</f>
         <v>0</v>
       </c>
       <c r="M65" s="1">
-        <f t="shared" si="12"/>
+        <f>M20+M18+M5</f>
         <v>1300</v>
       </c>
       <c r="N65" s="1">
@@ -3647,7 +3650,7 @@
         <v>15.6</v>
       </c>
       <c r="Q65" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>0.38400000000000001</v>
       </c>
       <c r="R65" s="1">
@@ -3655,56 +3658,56 @@
         <v>154.9</v>
       </c>
       <c r="S65" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>964.7</v>
       </c>
     </row>
     <row r="66" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B66" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C66" s="1">
-        <f t="shared" ref="C66:M66" si="13">C24+C23+C21+C5</f>
+        <f>C24+C23+C21+C5</f>
         <v>16</v>
       </c>
       <c r="D66" s="1">
-        <f t="shared" si="13"/>
+        <f>D24+D23+D21+D5</f>
         <v>0.38</v>
       </c>
       <c r="E66" s="1">
-        <f t="shared" si="13"/>
+        <f>E24+E23+E21+E5</f>
         <v>-10</v>
       </c>
       <c r="F66" s="1">
-        <f t="shared" si="13"/>
+        <f>F24+F23+F21+F5</f>
         <v>-10</v>
       </c>
       <c r="G66" s="1">
-        <f t="shared" si="13"/>
+        <f>G24+G23+G21+G5</f>
         <v>0</v>
       </c>
       <c r="H66" s="1">
-        <f t="shared" si="13"/>
+        <f>H24+H23+H21+H5</f>
         <v>0</v>
       </c>
       <c r="I66" s="1">
-        <f t="shared" si="13"/>
+        <f>I24+I23+I21+I5</f>
         <v>0</v>
       </c>
       <c r="J66" s="1">
-        <f t="shared" si="13"/>
+        <f>J24+J23+J21+J5</f>
         <v>0</v>
       </c>
       <c r="K66" s="1">
-        <f t="shared" si="13"/>
+        <f>K24+K23+K21+K5</f>
         <v>0</v>
       </c>
       <c r="L66" s="1">
-        <f t="shared" si="13"/>
+        <f>L24+L23+L21+L5</f>
         <v>0</v>
       </c>
       <c r="M66" s="1">
-        <f t="shared" si="13"/>
+        <f>M24+M23+M21+M5</f>
         <v>1000</v>
       </c>
       <c r="N66" s="1">
@@ -3716,7 +3719,7 @@
         <v>20</v>
       </c>
       <c r="Q66" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>0.44999999999999996</v>
       </c>
       <c r="R66" s="1">
@@ -3724,56 +3727,56 @@
         <v>244.99</v>
       </c>
       <c r="S66" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1234.97</v>
       </c>
     </row>
     <row r="67" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B67" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C67" s="1">
-        <f t="shared" ref="C67:M67" si="14">C25+C21+C5</f>
+        <f>C25+C21+C5</f>
         <v>18</v>
       </c>
       <c r="D67" s="1">
-        <f t="shared" si="14"/>
+        <f>D25+D21+D5</f>
         <v>0.31000000000000005</v>
       </c>
       <c r="E67" s="1">
-        <f t="shared" si="14"/>
+        <f>E25+E21+E5</f>
         <v>-3</v>
       </c>
       <c r="F67" s="1">
-        <f t="shared" si="14"/>
+        <f>F25+F21+F5</f>
         <v>-3</v>
       </c>
       <c r="G67" s="1">
-        <f t="shared" si="14"/>
+        <f>G25+G21+G5</f>
         <v>0</v>
       </c>
       <c r="H67" s="1">
-        <f t="shared" si="14"/>
+        <f>H25+H21+H5</f>
         <v>0</v>
       </c>
       <c r="I67" s="1">
-        <f t="shared" si="14"/>
+        <f>I25+I21+I5</f>
         <v>0</v>
       </c>
       <c r="J67" s="1">
-        <f t="shared" si="14"/>
+        <f>J25+J21+J5</f>
         <v>0</v>
       </c>
       <c r="K67" s="1">
-        <f t="shared" si="14"/>
+        <f>K25+K21+K5</f>
         <v>0</v>
       </c>
       <c r="L67" s="1">
-        <f t="shared" si="14"/>
+        <f>L25+L21+L5</f>
         <v>0</v>
       </c>
       <c r="M67" s="1">
-        <f t="shared" si="14"/>
+        <f>M25+M21+M5</f>
         <v>500</v>
       </c>
       <c r="N67" s="1">
@@ -3785,7 +3788,7 @@
         <v>15.4</v>
       </c>
       <c r="Q67" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>0.38100000000000001</v>
       </c>
       <c r="R67" s="1">
@@ -3793,60 +3796,60 @@
         <v>0</v>
       </c>
       <c r="S67" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>500</v>
       </c>
     </row>
     <row r="68" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B68" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C68" s="1">
-        <f t="shared" ref="C68:M68" si="15">C29+C26+C21+C5</f>
+        <f>C29+C26+C21+C5</f>
         <v>16</v>
       </c>
       <c r="D68" s="1">
-        <f t="shared" si="15"/>
+        <f>D29+D26+D21+D5</f>
         <v>0.34</v>
       </c>
       <c r="E68" s="1">
-        <f t="shared" si="15"/>
+        <f>E29+E26+E21+E5</f>
         <v>-13</v>
       </c>
       <c r="F68" s="1">
-        <f t="shared" si="15"/>
+        <f>F29+F26+F21+F5</f>
         <v>-7</v>
       </c>
       <c r="G68" s="1">
-        <f t="shared" si="15"/>
+        <f>G29+G26+G21+G5</f>
         <v>0</v>
       </c>
       <c r="H68" s="1">
-        <f t="shared" si="15"/>
+        <f>H29+H26+H21+H5</f>
         <v>0</v>
       </c>
       <c r="I68" s="1">
-        <f t="shared" si="15"/>
+        <f>I29+I26+I21+I5</f>
         <v>0</v>
       </c>
       <c r="J68" s="1">
-        <f t="shared" si="15"/>
+        <f>J29+J26+J21+J5</f>
         <v>0</v>
       </c>
       <c r="K68" s="1">
-        <f t="shared" si="15"/>
+        <f>K29+K26+K21+K5</f>
         <v>0</v>
       </c>
       <c r="L68" s="1">
-        <f t="shared" si="15"/>
+        <f>L29+L26+L21+L5</f>
         <v>0</v>
       </c>
       <c r="M68" s="1">
-        <f t="shared" si="15"/>
+        <f>M29+M26+M21+M5</f>
         <v>1500</v>
       </c>
       <c r="N68" s="1">
-        <f t="shared" ref="N68:N82" si="16">C68-(D68*20)-(E68*0.8)-(F68*0.6)-(H68*5)</f>
+        <f t="shared" ref="N68:N82" si="4">C68-(D68*20)-(E68*0.8)-(F68*0.6)-(H68*5)</f>
         <v>23.8</v>
       </c>
       <c r="P68" s="1">
@@ -3854,7 +3857,7 @@
         <v>20.6</v>
       </c>
       <c r="Q68" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>0.45899999999999996</v>
       </c>
       <c r="R68" s="1">
@@ -3862,60 +3865,60 @@
         <v>402.9</v>
       </c>
       <c r="S68" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1708.6999999999998</v>
       </c>
     </row>
     <row r="69" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B69" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C69" s="1">
-        <f t="shared" ref="C69:M69" si="17">C30+C26+C21+C5</f>
+        <f>C30+C26+C21+C5</f>
         <v>15</v>
       </c>
       <c r="D69" s="1">
-        <f t="shared" si="17"/>
+        <f>D30+D26+D21+D5</f>
         <v>0.4</v>
       </c>
       <c r="E69" s="1">
-        <f t="shared" si="17"/>
+        <f>E30+E26+E21+E5</f>
         <v>-6</v>
       </c>
       <c r="F69" s="1">
-        <f t="shared" si="17"/>
+        <f>F30+F26+F21+F5</f>
         <v>-20</v>
       </c>
       <c r="G69" s="1">
-        <f t="shared" si="17"/>
+        <f>G30+G26+G21+G5</f>
         <v>0</v>
       </c>
       <c r="H69" s="1">
-        <f t="shared" si="17"/>
+        <f>H30+H26+H21+H5</f>
         <v>0</v>
       </c>
       <c r="I69" s="1">
-        <f t="shared" si="17"/>
+        <f>I30+I26+I21+I5</f>
         <v>0</v>
       </c>
       <c r="J69" s="1">
-        <f t="shared" si="17"/>
+        <f>J30+J26+J21+J5</f>
         <v>0</v>
       </c>
       <c r="K69" s="1">
-        <f t="shared" si="17"/>
+        <f>K30+K26+K21+K5</f>
         <v>0</v>
       </c>
       <c r="L69" s="1">
-        <f t="shared" si="17"/>
+        <f>L30+L26+L21+L5</f>
         <v>0</v>
       </c>
       <c r="M69" s="1">
-        <f t="shared" si="17"/>
+        <f>M30+M26+M21+M5</f>
         <v>1600</v>
       </c>
       <c r="N69" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="4"/>
         <v>23.8</v>
       </c>
       <c r="P69" s="1">
@@ -3923,7 +3926,7 @@
         <v>17.8</v>
       </c>
       <c r="Q69" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>0.41700000000000004</v>
       </c>
       <c r="R69" s="1">
@@ -3931,60 +3934,60 @@
         <v>302.89999999999998</v>
       </c>
       <c r="S69" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1408.6999999999998</v>
       </c>
     </row>
     <row r="70" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B70" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C70" s="1">
-        <f t="shared" ref="C70:M70" si="18">C31+C32+C26+C21+C5</f>
+        <f>C31+C32+C26+C21+C5</f>
         <v>18</v>
       </c>
       <c r="D70" s="1">
-        <f t="shared" si="18"/>
+        <f>D31+D32+D26+D21+D5</f>
         <v>0.30000000000000004</v>
       </c>
       <c r="E70" s="1">
-        <f t="shared" si="18"/>
+        <f>E31+E32+E26+E21+E5</f>
         <v>-8</v>
       </c>
       <c r="F70" s="1">
-        <f t="shared" si="18"/>
+        <f>F31+F32+F26+F21+F5</f>
         <v>-9</v>
       </c>
       <c r="G70" s="1">
-        <f t="shared" si="18"/>
+        <f>G31+G32+G26+G21+G5</f>
         <v>0</v>
       </c>
       <c r="H70" s="1">
-        <f t="shared" si="18"/>
+        <f>H31+H32+H26+H21+H5</f>
         <v>0</v>
       </c>
       <c r="I70" s="1">
-        <f t="shared" si="18"/>
+        <f>I31+I32+I26+I21+I5</f>
         <v>0</v>
       </c>
       <c r="J70" s="1">
-        <f t="shared" si="18"/>
+        <f>J31+J32+J26+J21+J5</f>
         <v>0</v>
       </c>
       <c r="K70" s="1">
-        <f t="shared" si="18"/>
+        <f>K31+K32+K26+K21+K5</f>
         <v>0</v>
       </c>
       <c r="L70" s="1">
-        <f t="shared" si="18"/>
+        <f>L31+L32+L26+L21+L5</f>
         <v>0</v>
       </c>
       <c r="M70" s="1">
-        <f t="shared" si="18"/>
+        <f>M31+M32+M26+M21+M5</f>
         <v>1100</v>
       </c>
       <c r="N70" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="4"/>
         <v>23.799999999999997</v>
       </c>
       <c r="P70" s="1">
@@ -3992,7 +3995,7 @@
         <v>11.399999999999999</v>
       </c>
       <c r="Q70" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>0.32099999999999995</v>
       </c>
       <c r="R70" s="1">
@@ -4000,60 +4003,60 @@
         <v>98.9</v>
       </c>
       <c r="S70" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>796.7</v>
       </c>
     </row>
     <row r="71" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B71" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C71" s="1">
-        <f t="shared" ref="C71:M71" si="19">C34+C33+C26+C21+C5</f>
+        <f>C34+C33+C26+C21+C5</f>
         <v>17</v>
       </c>
       <c r="D71" s="1">
-        <f t="shared" si="19"/>
+        <f>D34+D33+D26+D21+D5</f>
         <v>0.35000000000000003</v>
       </c>
       <c r="E71" s="1">
-        <f t="shared" si="19"/>
+        <f>E34+E33+E26+E21+E5</f>
         <v>-11</v>
       </c>
       <c r="F71" s="1">
-        <f t="shared" si="19"/>
+        <f>F34+F33+F26+F21+F5</f>
         <v>-10</v>
       </c>
       <c r="G71" s="1">
-        <f t="shared" si="19"/>
+        <f>G34+G33+G26+G21+G5</f>
         <v>0</v>
       </c>
       <c r="H71" s="1">
-        <f t="shared" si="19"/>
+        <f>H34+H33+H26+H21+H5</f>
         <v>0</v>
       </c>
       <c r="I71" s="1">
-        <f t="shared" si="19"/>
+        <f>I34+I33+I26+I21+I5</f>
         <v>0</v>
       </c>
       <c r="J71" s="1">
-        <f t="shared" si="19"/>
+        <f>J34+J33+J26+J21+J5</f>
         <v>0</v>
       </c>
       <c r="K71" s="1">
-        <f t="shared" si="19"/>
+        <f>K34+K33+K26+K21+K5</f>
         <v>0</v>
       </c>
       <c r="L71" s="1">
-        <f t="shared" si="19"/>
+        <f>L34+L33+L26+L21+L5</f>
         <v>0</v>
       </c>
       <c r="M71" s="1">
-        <f t="shared" si="19"/>
+        <f>M34+M33+M26+M21+M5</f>
         <v>1400</v>
       </c>
       <c r="N71" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="4"/>
         <v>24.8</v>
       </c>
       <c r="P71" s="1">
@@ -4061,7 +4064,7 @@
         <v>13.2</v>
       </c>
       <c r="Q71" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>0.34799999999999998</v>
       </c>
       <c r="R71" s="1">
@@ -4069,60 +4072,60 @@
         <v>97.9</v>
       </c>
       <c r="S71" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>793.7</v>
       </c>
     </row>
     <row r="72" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B72" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C72" s="1">
-        <f t="shared" ref="C72:M72" si="20">C36+C35+C26+C21+C5</f>
+        <f>C36+C35+C26+C21+C5</f>
         <v>16</v>
       </c>
       <c r="D72" s="1">
-        <f t="shared" si="20"/>
+        <f>D36+D35+D26+D21+D5</f>
         <v>0.39</v>
       </c>
       <c r="E72" s="1">
-        <f t="shared" si="20"/>
+        <f>E36+E35+E26+E21+E5</f>
         <v>-9</v>
       </c>
       <c r="F72" s="1">
-        <f t="shared" si="20"/>
+        <f>F36+F35+F26+F21+F5</f>
         <v>-14</v>
       </c>
       <c r="G72" s="1">
-        <f t="shared" si="20"/>
+        <f>G36+G35+G26+G21+G5</f>
         <v>0</v>
       </c>
       <c r="H72" s="1">
-        <f t="shared" si="20"/>
+        <f>H36+H35+H26+H21+H5</f>
         <v>0</v>
       </c>
       <c r="I72" s="1">
-        <f t="shared" si="20"/>
+        <f>I36+I35+I26+I21+I5</f>
         <v>0</v>
       </c>
       <c r="J72" s="1">
-        <f t="shared" si="20"/>
+        <f>J36+J35+J26+J21+J5</f>
         <v>0</v>
       </c>
       <c r="K72" s="1">
-        <f t="shared" si="20"/>
+        <f>K36+K35+K26+K21+K5</f>
         <v>0</v>
       </c>
       <c r="L72" s="1">
-        <f t="shared" si="20"/>
+        <f>L36+L35+L26+L21+L5</f>
         <v>0</v>
       </c>
       <c r="M72" s="1">
-        <f t="shared" si="20"/>
+        <f>M36+M35+M26+M21+M5</f>
         <v>1400</v>
       </c>
       <c r="N72" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="4"/>
         <v>23.799999999999997</v>
       </c>
       <c r="P72" s="1">
@@ -4130,7 +4133,7 @@
         <v>20.3</v>
       </c>
       <c r="Q72" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>0.45450000000000002</v>
       </c>
       <c r="R72" s="1">
@@ -4138,60 +4141,60 @@
         <v>302.95</v>
       </c>
       <c r="S72" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1408.85</v>
       </c>
     </row>
     <row r="73" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B73" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C73" s="1">
-        <f t="shared" ref="C73:M73" si="21">C38+C37+C26+C21+C5</f>
+        <f>C38+C37+C26+C21+C5</f>
         <v>14</v>
       </c>
       <c r="D73" s="1">
-        <f t="shared" si="21"/>
+        <f>D38+D37+D26+D21+D5</f>
         <v>0.42500000000000004</v>
       </c>
       <c r="E73" s="1">
-        <f t="shared" si="21"/>
+        <f>E38+E37+E26+E21+E5</f>
         <v>-12</v>
       </c>
       <c r="F73" s="1">
-        <f t="shared" si="21"/>
+        <f>F38+F37+F26+F21+F5</f>
         <v>-13</v>
       </c>
       <c r="G73" s="1">
-        <f t="shared" si="21"/>
+        <f>G38+G37+G26+G21+G5</f>
         <v>0</v>
       </c>
       <c r="H73" s="1">
-        <f t="shared" si="21"/>
+        <f>H38+H37+H26+H21+H5</f>
         <v>0</v>
       </c>
       <c r="I73" s="1">
-        <f t="shared" si="21"/>
+        <f>I38+I37+I26+I21+I5</f>
         <v>0</v>
       </c>
       <c r="J73" s="1">
-        <f t="shared" si="21"/>
+        <f>J38+J37+J26+J21+J5</f>
         <v>0</v>
       </c>
       <c r="K73" s="1">
-        <f t="shared" si="21"/>
+        <f>K38+K37+K26+K21+K5</f>
         <v>0</v>
       </c>
       <c r="L73" s="1">
-        <f t="shared" si="21"/>
+        <f>L38+L37+L26+L21+L5</f>
         <v>0</v>
       </c>
       <c r="M73" s="1">
-        <f t="shared" si="21"/>
+        <f>M38+M37+M26+M21+M5</f>
         <v>1300</v>
       </c>
       <c r="N73" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="4"/>
         <v>22.900000000000002</v>
       </c>
       <c r="P73" s="1">
@@ -4199,7 +4202,7 @@
         <v>18.8</v>
       </c>
       <c r="Q73" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>0.43199999999999994</v>
       </c>
       <c r="R73" s="1">
@@ -4207,59 +4210,59 @@
         <v>250.89999999999998</v>
       </c>
       <c r="S73" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1252.6999999999998</v>
       </c>
     </row>
     <row r="74" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B74" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C74" s="1">
-        <f t="shared" ref="C74:M74" si="22">C41+C40+C39+C26+C21+C5</f>
+        <f>C41+C40+C39+C26+C21+C5</f>
         <v>20</v>
       </c>
       <c r="D74" s="1">
-        <f t="shared" si="22"/>
+        <f>D41+D40+D39+D26+D21+D5</f>
         <v>0.56000000000000005</v>
       </c>
       <c r="E74" s="1">
-        <f t="shared" si="22"/>
+        <f>E41+E40+E39+E26+E21+E5</f>
         <v>-6</v>
       </c>
       <c r="F74" s="1">
         <v>-4</v>
       </c>
       <c r="G74" s="1">
-        <f t="shared" si="22"/>
+        <f>G41+G40+G39+G26+G21+G5</f>
         <v>0</v>
       </c>
       <c r="H74" s="1">
-        <f t="shared" si="22"/>
+        <f>H41+H40+H39+H26+H21+H5</f>
         <v>-0.1</v>
       </c>
       <c r="I74" s="1">
-        <f t="shared" si="22"/>
+        <f>I41+I40+I39+I26+I21+I5</f>
         <v>0</v>
       </c>
       <c r="J74" s="1">
-        <f t="shared" si="22"/>
+        <f>J41+J40+J39+J26+J21+J5</f>
         <v>0</v>
       </c>
       <c r="K74" s="1">
-        <f t="shared" si="22"/>
+        <f>K41+K40+K39+K26+K21+K5</f>
         <v>0</v>
       </c>
       <c r="L74" s="1">
-        <f t="shared" si="22"/>
+        <f>L41+L40+L39+L26+L21+L5</f>
         <v>0</v>
       </c>
       <c r="M74" s="1">
-        <f t="shared" si="22"/>
+        <f>M41+M40+M39+M26+M21+M5</f>
         <v>2100</v>
       </c>
       <c r="N74" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="4"/>
         <v>16.5</v>
       </c>
       <c r="P74" s="1">
@@ -4267,7 +4270,7 @@
         <v>32.6</v>
       </c>
       <c r="Q74" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>0.63900000000000001</v>
       </c>
       <c r="R74" s="1">
@@ -4275,60 +4278,60 @@
         <v>312.89999999999998</v>
       </c>
       <c r="S74" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1438.6999999999998</v>
       </c>
     </row>
     <row r="75" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B75" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C75" s="1">
-        <f t="shared" ref="C75:M75" si="23">C42+C26+C21+C5</f>
+        <f>C42+C26+C21+C5</f>
         <v>14</v>
       </c>
       <c r="D75" s="1">
-        <f t="shared" si="23"/>
+        <f>D42+D26+D21+D5</f>
         <v>0.35000000000000003</v>
       </c>
       <c r="E75" s="1">
-        <f t="shared" si="23"/>
+        <f>E42+E26+E21+E5</f>
         <v>-10</v>
       </c>
       <c r="F75" s="1">
-        <f t="shared" si="23"/>
+        <f>F42+F26+F21+F5</f>
         <v>-13</v>
       </c>
       <c r="G75" s="1">
-        <f t="shared" si="23"/>
+        <f>G42+G26+G21+G5</f>
         <v>0</v>
       </c>
       <c r="H75" s="1">
-        <f t="shared" si="23"/>
+        <f>H42+H26+H21+H5</f>
         <v>0</v>
       </c>
       <c r="I75" s="1">
-        <f t="shared" si="23"/>
+        <f>I42+I26+I21+I5</f>
         <v>0</v>
       </c>
       <c r="J75" s="1">
-        <f t="shared" si="23"/>
+        <f>J42+J26+J21+J5</f>
         <v>0</v>
       </c>
       <c r="K75" s="1">
-        <f t="shared" si="23"/>
+        <f>K42+K26+K21+K5</f>
         <v>0</v>
       </c>
       <c r="L75" s="1">
-        <f t="shared" si="23"/>
+        <f>L42+L26+L21+L5</f>
         <v>0</v>
       </c>
       <c r="M75" s="1">
-        <f t="shared" si="23"/>
+        <f>M42+M26+M21+M5</f>
         <v>1200</v>
       </c>
       <c r="N75" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="4"/>
         <v>22.8</v>
       </c>
       <c r="P75" s="1">
@@ -4336,7 +4339,7 @@
         <v>14.3</v>
       </c>
       <c r="Q75" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>0.36449999999999999</v>
       </c>
       <c r="R75" s="1">
@@ -4344,60 +4347,60 @@
         <v>112.85</v>
       </c>
       <c r="S75" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>838.55</v>
       </c>
     </row>
     <row r="76" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B76" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C76" s="1">
-        <f t="shared" ref="C76:M76" si="24">C43+C26+C21+C5</f>
+        <f>C43+C26+C21+C5</f>
         <v>15</v>
       </c>
       <c r="D76" s="1">
-        <f t="shared" si="24"/>
+        <f>D43+D26+D21+D5</f>
         <v>0.36000000000000004</v>
       </c>
       <c r="E76" s="1">
-        <f t="shared" si="24"/>
+        <f>E43+E26+E21+E5</f>
         <v>-13</v>
       </c>
       <c r="F76" s="1">
-        <f t="shared" si="24"/>
+        <f>F43+F26+F21+F5</f>
         <v>-8</v>
       </c>
       <c r="G76" s="1">
-        <f t="shared" si="24"/>
+        <f>G43+G26+G21+G5</f>
         <v>0</v>
       </c>
       <c r="H76" s="1">
-        <f t="shared" si="24"/>
+        <f>H43+H26+H21+H5</f>
         <v>0</v>
       </c>
       <c r="I76" s="1">
-        <f t="shared" si="24"/>
+        <f>I43+I26+I21+I5</f>
         <v>0</v>
       </c>
       <c r="J76" s="1">
-        <f t="shared" si="24"/>
+        <f>J43+J26+J21+J5</f>
         <v>0</v>
       </c>
       <c r="K76" s="1">
-        <f t="shared" si="24"/>
+        <f>K43+K26+K21+K5</f>
         <v>0</v>
       </c>
       <c r="L76" s="1">
-        <f t="shared" si="24"/>
+        <f>L43+L26+L21+L5</f>
         <v>0</v>
       </c>
       <c r="M76" s="1">
-        <f t="shared" si="24"/>
+        <f>M43+M26+M21+M5</f>
         <v>1350</v>
       </c>
       <c r="N76" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="4"/>
         <v>23</v>
       </c>
       <c r="P76" s="1">
@@ -4405,7 +4408,7 @@
         <v>14.8</v>
       </c>
       <c r="Q76" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>0.372</v>
       </c>
       <c r="R76" s="1">
@@ -4413,60 +4416,60 @@
         <v>52.95</v>
       </c>
       <c r="S76" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>658.85</v>
       </c>
     </row>
     <row r="77" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B77" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C77" s="1">
-        <f t="shared" ref="C77:M77" si="25">C44+C26+C21+C5</f>
+        <f>C44+C26+C21+C5</f>
         <v>15</v>
       </c>
       <c r="D77" s="1">
-        <f t="shared" si="25"/>
+        <f>D44+D26+D21+D5</f>
         <v>0.34</v>
       </c>
       <c r="E77" s="1">
-        <f t="shared" si="25"/>
+        <f>E44+E26+E21+E5</f>
         <v>-10</v>
       </c>
       <c r="F77" s="1">
-        <f t="shared" si="25"/>
+        <f>F44+F26+F21+F5</f>
         <v>-8</v>
       </c>
       <c r="G77" s="1">
-        <f t="shared" si="25"/>
+        <f>G44+G26+G21+G5</f>
         <v>0</v>
       </c>
       <c r="H77" s="1">
-        <f t="shared" si="25"/>
+        <f>H44+H26+H21+H5</f>
         <v>0</v>
       </c>
       <c r="I77" s="1">
-        <f t="shared" si="25"/>
+        <f>I44+I26+I21+I5</f>
         <v>0</v>
       </c>
       <c r="J77" s="1">
-        <f t="shared" si="25"/>
+        <f>J44+J26+J21+J5</f>
         <v>0</v>
       </c>
       <c r="K77" s="1">
-        <f t="shared" si="25"/>
+        <f>K44+K26+K21+K5</f>
         <v>0</v>
       </c>
       <c r="L77" s="1">
-        <f t="shared" si="25"/>
+        <f>L44+L26+L21+L5</f>
         <v>0</v>
       </c>
       <c r="M77" s="1">
-        <f t="shared" si="25"/>
+        <f>M44+M26+M21+M5</f>
         <v>600</v>
       </c>
       <c r="N77" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="4"/>
         <v>21</v>
       </c>
       <c r="P77" s="1">
@@ -4474,7 +4477,7 @@
         <v>12.8</v>
       </c>
       <c r="Q77" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>0.34199999999999997</v>
       </c>
       <c r="R77" s="1">
@@ -4482,60 +4485,60 @@
         <v>52.95</v>
       </c>
       <c r="S77" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>658.85</v>
       </c>
     </row>
     <row r="78" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B78" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C78" s="1">
-        <f t="shared" ref="C78:M78" si="26">C46+C45+C26+C21+C5</f>
+        <f>C46+C45+C26+C21+C5</f>
         <v>18</v>
       </c>
       <c r="D78" s="1">
-        <f t="shared" si="26"/>
+        <f>D46+D45+D26+D21+D5</f>
         <v>0.4</v>
       </c>
       <c r="E78" s="1">
-        <f t="shared" si="26"/>
+        <f>E46+E45+E26+E21+E5</f>
         <v>-7</v>
       </c>
       <c r="F78" s="1">
-        <f t="shared" si="26"/>
+        <f>F46+F45+F26+F21+F5</f>
         <v>-15</v>
       </c>
       <c r="G78" s="1">
-        <f t="shared" si="26"/>
+        <f>G46+G45+G26+G21+G5</f>
         <v>0</v>
       </c>
       <c r="H78" s="1">
-        <f t="shared" si="26"/>
+        <f>H46+H45+H26+H21+H5</f>
         <v>0</v>
       </c>
       <c r="I78" s="1">
-        <f t="shared" si="26"/>
+        <f>I46+I45+I26+I21+I5</f>
         <v>0</v>
       </c>
       <c r="J78" s="1">
-        <f t="shared" si="26"/>
+        <f>J46+J45+J26+J21+J5</f>
         <v>0</v>
       </c>
       <c r="K78" s="1">
-        <f t="shared" si="26"/>
+        <f>K46+K45+K26+K21+K5</f>
         <v>0</v>
       </c>
       <c r="L78" s="1">
-        <f t="shared" si="26"/>
+        <f>L46+L45+L26+L21+L5</f>
         <v>0</v>
       </c>
       <c r="M78" s="1">
-        <f t="shared" si="26"/>
+        <f>M46+M45+M26+M21+M5</f>
         <v>1300</v>
       </c>
       <c r="N78" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="4"/>
         <v>24.6</v>
       </c>
       <c r="P78" s="1">
@@ -4543,7 +4546,7 @@
         <v>17.2</v>
       </c>
       <c r="Q78" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>0.40800000000000003</v>
       </c>
       <c r="R78" s="1">
@@ -4551,60 +4554,60 @@
         <v>261.95</v>
       </c>
       <c r="S78" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1285.8499999999999</v>
       </c>
     </row>
     <row r="79" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B79" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C79" s="1">
-        <f t="shared" ref="C79:M79" si="27">C48+C47+C26+C21+C5</f>
+        <f>C48+C47+C26+C21+C5</f>
         <v>16</v>
       </c>
       <c r="D79" s="1">
-        <f t="shared" si="27"/>
+        <f>D48+D47+D26+D21+D5</f>
         <v>0.31000000000000005</v>
       </c>
       <c r="E79" s="1">
-        <f t="shared" si="27"/>
+        <f>E48+E47+E26+E21+E5</f>
         <v>-8</v>
       </c>
       <c r="F79" s="1">
-        <f t="shared" si="27"/>
+        <f>F48+F47+F26+F21+F5</f>
         <v>-13</v>
       </c>
       <c r="G79" s="1">
-        <f t="shared" si="27"/>
+        <f>G48+G47+G26+G21+G5</f>
         <v>0</v>
       </c>
       <c r="H79" s="1">
-        <f t="shared" si="27"/>
+        <f>H48+H47+H26+H21+H5</f>
         <v>0</v>
       </c>
       <c r="I79" s="1">
-        <f t="shared" si="27"/>
+        <f>I48+I47+I26+I21+I5</f>
         <v>0</v>
       </c>
       <c r="J79" s="1">
-        <f t="shared" si="27"/>
+        <f>J48+J47+J26+J21+J5</f>
         <v>0</v>
       </c>
       <c r="K79" s="1">
-        <f t="shared" si="27"/>
+        <f>K48+K47+K26+K21+K5</f>
         <v>0</v>
       </c>
       <c r="L79" s="1">
-        <f t="shared" si="27"/>
+        <f>L48+L47+L26+L21+L5</f>
         <v>0</v>
       </c>
       <c r="M79" s="1">
-        <f t="shared" si="27"/>
+        <f>M48+M47+M26+M21+M5</f>
         <v>1100</v>
       </c>
       <c r="N79" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="4"/>
         <v>24</v>
       </c>
       <c r="P79" s="1">
@@ -4612,7 +4615,7 @@
         <v>10.399999999999999</v>
       </c>
       <c r="Q79" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>0.30599999999999994</v>
       </c>
       <c r="R79" s="1">
@@ -4620,60 +4623,60 @@
         <v>102.95</v>
       </c>
       <c r="S79" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>808.85</v>
       </c>
     </row>
     <row r="80" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B80" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C80" s="1">
-        <f t="shared" ref="C80:M80" si="28">C50+C49+C26+C21+C5</f>
+        <f>C50+C49+C26+C21+C5</f>
         <v>17</v>
       </c>
       <c r="D80" s="1">
-        <f t="shared" si="28"/>
+        <f>D50+D49+D26+D21+D5</f>
         <v>0.39</v>
       </c>
       <c r="E80" s="1">
-        <f t="shared" si="28"/>
+        <f>E50+E49+E26+E21+E5</f>
         <v>-11</v>
       </c>
       <c r="F80" s="1">
-        <f t="shared" si="28"/>
+        <f>F50+F49+F26+F21+F5</f>
         <v>-11</v>
       </c>
       <c r="G80" s="1">
-        <f t="shared" si="28"/>
+        <f>G50+G49+G26+G21+G5</f>
         <v>0</v>
       </c>
       <c r="H80" s="1">
-        <f t="shared" si="28"/>
+        <f>H50+H49+H26+H21+H5</f>
         <v>0</v>
       </c>
       <c r="I80" s="1">
-        <f t="shared" si="28"/>
+        <f>I50+I49+I26+I21+I5</f>
         <v>0</v>
       </c>
       <c r="J80" s="1">
-        <f t="shared" si="28"/>
+        <f>J50+J49+J26+J21+J5</f>
         <v>0</v>
       </c>
       <c r="K80" s="1">
-        <f t="shared" si="28"/>
+        <f>K50+K49+K26+K21+K5</f>
         <v>0</v>
       </c>
       <c r="L80" s="1">
-        <f t="shared" si="28"/>
+        <f>L50+L49+L26+L21+L5</f>
         <v>0</v>
       </c>
       <c r="M80" s="1">
-        <f t="shared" si="28"/>
+        <f>M50+M49+M26+M21+M5</f>
         <v>1500</v>
       </c>
       <c r="N80" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="4"/>
         <v>24.6</v>
       </c>
       <c r="P80" s="1">
@@ -4681,7 +4684,7 @@
         <v>17.399999999999999</v>
       </c>
       <c r="Q80" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>0.41099999999999992</v>
       </c>
       <c r="R80" s="1">
@@ -4689,145 +4692,145 @@
         <v>137.9</v>
       </c>
       <c r="S80" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>913.7</v>
       </c>
     </row>
     <row r="81" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B81" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C81" s="1">
-        <f t="shared" ref="C81:L81" si="29">C52+C51+C26+C21+C5</f>
+        <f>C52+C51+C26+C21+C5</f>
         <v>18</v>
       </c>
       <c r="D81" s="1">
-        <f t="shared" si="29"/>
+        <f>D52+D51+D26+D21+D5</f>
         <v>0.33</v>
       </c>
       <c r="E81" s="1">
-        <f t="shared" si="29"/>
+        <f>E52+E51+E26+E21+E5</f>
         <v>-9</v>
       </c>
       <c r="F81" s="1">
-        <f t="shared" si="29"/>
+        <f>F52+F51+F26+F21+F5</f>
         <v>-10</v>
       </c>
       <c r="G81" s="1">
-        <f t="shared" si="29"/>
+        <f>G52+G51+G26+G21+G5</f>
         <v>0</v>
       </c>
       <c r="H81" s="1">
-        <f t="shared" si="29"/>
+        <f>H52+H51+H26+H21+H5</f>
         <v>0</v>
       </c>
       <c r="I81" s="1">
-        <f t="shared" si="29"/>
+        <f>I52+I51+I26+I21+I5</f>
         <v>0</v>
       </c>
       <c r="J81" s="1">
-        <f t="shared" si="29"/>
+        <f>J52+J51+J26+J21+J5</f>
         <v>0</v>
       </c>
       <c r="K81" s="1">
-        <f t="shared" si="29"/>
+        <f>K52+K51+K26+K21+K5</f>
         <v>0</v>
       </c>
       <c r="L81" s="1">
-        <f t="shared" si="29"/>
+        <f>L52+L51+L26+L21+L5</f>
         <v>0</v>
       </c>
       <c r="M81" s="1">
-        <f t="shared" ref="M81:R81" si="30">M52+M51+M26+M21+M5</f>
+        <f>M52+M51+M26+M21+M5</f>
         <v>1400</v>
       </c>
       <c r="N81" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="4"/>
         <v>24.599999999999998</v>
       </c>
       <c r="P81" s="1">
-        <f t="shared" si="30"/>
+        <f>P52+P51+P26+P21+P5</f>
         <v>12.6</v>
       </c>
       <c r="Q81" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>0.33899999999999997</v>
       </c>
       <c r="R81" s="1">
-        <f t="shared" si="30"/>
+        <f>R52+R51+R26+R21+R5</f>
         <v>97.9</v>
       </c>
       <c r="S81" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>793.7</v>
       </c>
     </row>
     <row r="82" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B82" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C82" s="1">
         <f>C54+C53+C26+C21+C5</f>
         <v>16</v>
       </c>
       <c r="D82" s="1">
-        <f t="shared" ref="D82:R82" si="31">D54+D53+D26+D21+D5</f>
+        <f>D54+D53+D26+D21+D5</f>
         <v>0.34</v>
       </c>
       <c r="E82" s="1">
-        <f t="shared" si="31"/>
+        <f>E54+E53+E26+E21+E5</f>
         <v>-10</v>
       </c>
       <c r="F82" s="1">
-        <f t="shared" si="31"/>
+        <f>F54+F53+F26+F21+F5</f>
         <v>-12</v>
       </c>
       <c r="G82" s="1">
-        <f t="shared" si="31"/>
+        <f>G54+G53+G26+G21+G5</f>
         <v>0</v>
       </c>
       <c r="H82" s="1">
-        <f t="shared" si="31"/>
+        <f>H54+H53+H26+H21+H5</f>
         <v>0</v>
       </c>
       <c r="I82" s="1">
-        <f t="shared" si="31"/>
+        <f>I54+I53+I26+I21+I5</f>
         <v>0</v>
       </c>
       <c r="J82" s="1">
-        <f t="shared" si="31"/>
+        <f>J54+J53+J26+J21+J5</f>
         <v>0</v>
       </c>
       <c r="K82" s="1">
-        <f t="shared" si="31"/>
+        <f>K54+K53+K26+K21+K5</f>
         <v>0</v>
       </c>
       <c r="L82" s="1">
-        <f t="shared" si="31"/>
+        <f>L54+L53+L26+L21+L5</f>
         <v>0</v>
       </c>
       <c r="M82" s="1">
-        <f t="shared" si="31"/>
+        <f>M54+M53+M26+M21+M5</f>
         <v>1500</v>
       </c>
       <c r="N82" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="4"/>
         <v>24.4</v>
       </c>
       <c r="P82" s="1">
-        <f t="shared" si="31"/>
+        <f>P54+P53+P26+P21+P5</f>
         <v>12.8</v>
       </c>
       <c r="Q82" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>0.34199999999999997</v>
       </c>
       <c r="R82" s="1">
-        <f t="shared" si="31"/>
+        <f>R54+R53+R26+R21+R5</f>
         <v>134.94999999999999</v>
       </c>
       <c r="S82" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>904.84999999999991</v>
       </c>
     </row>

</xml_diff>